<commit_message>
scrol down and negative test
</commit_message>
<xml_diff>
--- a/src/main/java/com/asynctric/qa/testdata/AddressTestData.xlsx
+++ b/src/main/java/com/asynctric/qa/testdata/AddressTestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -111,13 +112,22 @@
   </si>
   <si>
     <t>9876543210</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>arun5603@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +139,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +190,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,8 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -502,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,4 +673,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>